<commit_message>
Added methionine genes and rxns but no growth
</commit_message>
<xml_diff>
--- a/Lit Sources/Methionine/methionine JL.xlsx
+++ b/Lit Sources/Methionine/methionine JL.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15576" windowHeight="9816" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -263,16 +263,21 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -600,13 +605,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="57" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,7 +628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -634,7 +642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -648,7 +656,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -662,7 +670,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -676,7 +684,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -690,7 +698,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -704,7 +712,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -718,13 +726,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -738,7 +746,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -749,7 +757,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -763,7 +771,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -777,7 +785,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -791,93 +799,93 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="3" t="s">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="B23" s="3" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
         <v>60</v>
       </c>
       <c r="D23" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="B24" s="3" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
         <v>62</v>
       </c>
       <c r="D24" t="s">

</xml_diff>